<commit_message>
remove hiper link from email link after remove email show in console
</commit_message>
<xml_diff>
--- a/EXCEL_FILE.xlsx
+++ b/EXCEL_FILE.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">ABOBAKAR</t>
   </si>
   <si>
-    <t xml:space="preserve">ranaabobakarit@gmail.com</t>
+    <t xml:space="preserve">ranaabobakar777@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">AOA</t>
@@ -46,13 +46,16 @@
     <t xml:space="preserve">SHAHZEB</t>
   </si>
   <si>
-    <t xml:space="preserve">19014156-022@uog.edu.pk</t>
-  </si>
-  <si>
     <t xml:space="preserve">ZEESHAN</t>
   </si>
   <si>
-    <t xml:space="preserve">ranaabobakar777@gmail.com</t>
+    <t xml:space="preserve">shan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shan@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WAS</t>
   </si>
 </sst>
 </file>
@@ -67,6 +70,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -88,6 +92,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -158,15 +163,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.62"/>
   </cols>
   <sheetData>
@@ -206,7 +211,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>6</v>
@@ -217,21 +222,30 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="ranaabobakarit@gmail.com"/>
-    <hyperlink ref="C3" r:id="rId2" display="19014156-022@uog.edu.pk"/>
-    <hyperlink ref="C4" r:id="rId3" display="ranaabobakar777@gmail.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
code write but not working
</commit_message>
<xml_diff>
--- a/EXCEL_FILE.xlsx
+++ b/EXCEL_FILE.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -37,25 +37,22 @@
     <t xml:space="preserve">ABOBAKAR</t>
   </si>
   <si>
+    <t xml:space="preserve">ranaabobakarit@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kya hal ha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHAHZEB</t>
+  </si>
+  <si>
     <t xml:space="preserve">ranaabobakar777@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">AOA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHAHZEB</t>
-  </si>
-  <si>
     <t xml:space="preserve">ZEESHAN</t>
   </si>
   <si>
-    <t xml:space="preserve">shan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shan@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WAS</t>
+    <t xml:space="preserve">abobakarit786@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -65,7 +62,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -93,6 +90,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,12 +139,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -163,16 +169,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -211,9 +218,9 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -222,27 +229,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>